<commit_message>
整理文件夹 Signed-off-by: anshu.wang <anshu.wang.work@gmail.com>
</commit_message>
<xml_diff>
--- a/writting/学科知识体系/计算机/文稿动画/presentation 要点.xlsx
+++ b/writting/学科知识体系/计算机/文稿动画/presentation 要点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="7595" activeTab="2"/>
+    <workbookView windowWidth="21600" windowHeight="10800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="分类" sheetId="2" r:id="rId1"/>
@@ -188,17 +188,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,22 +217,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -232,15 +226,96 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -248,15 +323,23 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -264,90 +347,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -367,187 +367,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,6 +558,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -580,7 +595,51 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -599,276 +658,220 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1139,27 +1142,27 @@
   <sheetPr/>
   <dimension ref="B4:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="2" max="2" width="52.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="52.7166666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" ht="16.8" spans="2:2">
-      <c r="B4" s="2" t="s">
+    <row r="4" ht="16.5" spans="2:2">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="16.8" spans="2:2">
-      <c r="B5" s="2" t="s">
+    <row r="5" ht="16.5" spans="2:2">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="16.8" spans="2:2">
-      <c r="B6" s="2" t="s">
+    <row r="6" ht="16.5" spans="2:2">
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1178,7 +1181,7 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1190,17 +1193,17 @@
   <sheetPr/>
   <dimension ref="A2:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="23.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="20.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="22.4444444444444" customWidth="1"/>
-    <col min="7" max="7" width="28.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="11.775" customWidth="1"/>
+    <col min="2" max="2" width="23.1083333333333" customWidth="1"/>
+    <col min="3" max="3" width="20.2833333333333" customWidth="1"/>
+    <col min="6" max="6" width="22.4416666666667" customWidth="1"/>
+    <col min="7" max="7" width="28.5583333333333" customWidth="1"/>
     <col min="12" max="12" width="13.3333333333333" customWidth="1"/>
     <col min="13" max="13" width="25.6666666666667" customWidth="1"/>
   </cols>
@@ -1217,7 +1220,7 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1225,7 +1228,7 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1258,10 +1261,10 @@
       </c>
     </row>
     <row r="7" spans="12:15">
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="2"/>
       <c r="O7" t="s">
         <v>18</v>
       </c>
@@ -1270,8 +1273,8 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1" t="s">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="P8" t="s">
@@ -1301,10 +1304,10 @@
       </c>
     </row>
     <row r="11" spans="12:17">
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="M11" s="2"/>
       <c r="Q11" t="s">
         <v>29</v>
       </c>
@@ -1313,8 +1316,8 @@
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1" t="s">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1419,6 +1422,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" display="https://cloudconvert.com/"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://pixabay.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>